<commit_message>
Update binary files for Input + Equipment image and Excel documents
</commit_message>
<xml_diff>
--- a/BandColorConvention/BandColorConvention.xlsx
+++ b/BandColorConvention/BandColorConvention.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TechnicalDocumentation\Assets\BandColorConvention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TechnicalDocumentation\BandColorConvention\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2448D76-61CE-4111-BD41-50CCF6C8CF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910EFE02-BCBF-424E-A695-C31B00FF2494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-28905" yWindow="7740" windowWidth="28740" windowHeight="7845" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Style" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Chad</t>
   </si>
@@ -110,12 +110,6 @@
     <t>Billy</t>
   </si>
   <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Upstage Right</t>
   </si>
   <si>
@@ -132,6 +126,15 @@
   </si>
   <si>
     <t>USL</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>DSR</t>
   </si>
 </sst>
 </file>
@@ -206,7 +209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,14 +581,14 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
   </cols>
@@ -642,71 +645,71 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>13</v>
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>